<commit_message>
added collaboration.R for analyze collaboration countries and institutions
</commit_message>
<xml_diff>
--- a/citations/works_cited_source_nonissn_brill.xlsx
+++ b/citations/works_cited_source_nonissn_brill.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL38"/>
+  <dimension ref="A1:AL50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,22 +552,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2999704425</t>
+          <t>https://openalex.org/W4251265902</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Two Functional Categories in Noun Phrases: Evidence from Modern Hebrew</t>
+          <t>W.H.O., The Global Eradication of Smallpox. Final Report of The Global Commission for the Certification of Smallpox Eradication. Geneva, World Health Organization, 1980, 122 pp., Sfr. 11,-.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Two Functional Categories in Noun Phrases: Evidence from Modern Hebrew</t>
+          <t>W.H.O., The Global Eradication of Smallpox. Final Report of The Global Commission for the Certification of Smallpox Eradication. Geneva, World Health Organization, 1980, 122 pp., Sfr. 11,-.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1991-12-26</t>
+          <t>1982-01-01</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -587,17 +587,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004373198_004</t>
+          <t>https://doi.org/10.1163/9789004418677_071</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>268</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>269</t>
         </is>
       </c>
       <c r="S2" t="b">
@@ -620,19 +620,19 @@
         </is>
       </c>
       <c r="Z2">
-        <v>647</v>
+        <v>3</v>
       </c>
       <c r="AB2">
-        <v>1991</v>
+        <v>1982</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2999704425</t>
+          <t>https://api.openalex.org/works?filter=cites:W4251265902</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004373198_004</t>
+          <t>https://doi.org/10.1163/9789004418677_071</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
@@ -650,27 +650,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2973152659</t>
+          <t>https://openalex.org/W2264742718</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4 History and Climate: The Crisis of the 1590s Reconsidered</t>
+          <t>Logic and Conversation</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4 History and Climate: The Crisis of the 1590s Reconsidered</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>In 1985, a book entitled The European Crisis of the 1590s: Essays in Comparative History, edited by Peter Clark, examined the experience of ten individual regions of Western Europe, eight of them ruled either by Philip II or by his principal enemies: Elizabeth Tudor, Henry IV of France, and the Dutch. Although the individual authors noted specific disasters, most concluded that the 1590s were merely one of the cyclical crises that afflicted premodern societies. Since then, the publication of data on the global climate reveals that the 1590s saw some of the worst weather ever recorded in the northern hemisphere, a severe episode in the "Little Ice Age"—an era of major volcanic eruptions, reduced solar activity, and multiple El Niño events—linked with an increased frequency of extreme climatic events, plague, famine, and war.</t>
+          <t>Logic and Conversation</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2018-01-01</t>
+          <t>1975-12-12</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -690,17 +685,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004356825_006</t>
+          <t>https://doi.org/10.1163/9789004368811_003</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>41</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>58</t>
         </is>
       </c>
       <c r="S3" t="b">
@@ -723,19 +718,19 @@
         </is>
       </c>
       <c r="Z3">
-        <v>14</v>
+        <v>19863</v>
       </c>
       <c r="AB3">
-        <v>2018</v>
+        <v>1975</v>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2973152659</t>
+          <t>https://api.openalex.org/works?filter=cites:W2264742718</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004356825_006</t>
+          <t>https://doi.org/10.1163/9789004368811_003</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
@@ -753,22 +748,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4245901630</t>
+          <t>https://openalex.org/W2776762211</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Human Development Reports</t>
+          <t>Ecospace Rights: Sharing or Dividing</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Human Development Reports</t>
+          <t>Ecospace Rights: Sharing or Dividing</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2010-01-01</t>
+          <t>1998-01-01</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -788,17 +783,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004180048.i-962.200</t>
+          <t>https://doi.org/10.1163/9789004633063_029</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>248</t>
+          <t>398</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>414</t>
         </is>
       </c>
       <c r="S4" t="b">
@@ -817,23 +812,23 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>nl</t>
+          <t>en</t>
         </is>
       </c>
       <c r="Z4">
-        <v>489</v>
+        <v>2</v>
       </c>
       <c r="AB4">
-        <v>2010</v>
+        <v>1998</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4245901630</t>
+          <t>https://api.openalex.org/works?filter=cites:W2776762211</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004180048.i-962.200</t>
+          <t>https://doi.org/10.1163/9789004633063_029</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
@@ -851,22 +846,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2600295159</t>
+          <t>https://openalex.org/W4361747929</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10 Revolts under the Ptolemies: A Paleoclimatological Perspective</t>
+          <t>The Ghost of the Counterfeit in the Genesis of the Gothic</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10 Revolts under the Ptolemies: A Paleoclimatological Perspective</t>
+          <t>The Ghost of the Counterfeit in the Genesis of the Gothic</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2016-01-01</t>
+          <t>1994-01-01</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -886,17 +881,17 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004330184_011</t>
+          <t>https://doi.org/10.1163/9789004483743_005</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>23</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>171</t>
+          <t>33</t>
         </is>
       </c>
       <c r="S5" t="b">
@@ -919,19 +914,19 @@
         </is>
       </c>
       <c r="Z5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AB5">
-        <v>2016</v>
+        <v>1994</v>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2600295159</t>
+          <t>https://api.openalex.org/works?filter=cites:W4361747929</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004330184_011</t>
+          <t>https://doi.org/10.1163/9789004483743_005</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
@@ -949,22 +944,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4387961581</t>
+          <t>https://openalex.org/W2924858335</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Studying Fossil Horses</t>
+          <t>Scientific Worldview Studies: A Programmatic Proposal</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Studying Fossil Horses</t>
+          <t>Scientific Worldview Studies: A Programmatic Proposal</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1988-01-01</t>
+          <t>2018-01-01</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -984,7 +979,17 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004675629</t>
+          <t>https://doi.org/10.1163/9789004385375_020</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>297</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>308</t>
         </is>
       </c>
       <c r="S6" t="b">
@@ -1001,25 +1006,30 @@
       <c r="W6" t="b">
         <v>0</v>
       </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
       <c r="Z6">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="AB6">
-        <v>1988</v>
+        <v>2018</v>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4387961581</t>
+          <t>https://api.openalex.org/works?filter=cites:W2924858335</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004675629</t>
+          <t>https://doi.org/10.1163/9789004385375_020</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI6" t="b">
@@ -1032,27 +1042,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://openalex.org/W955020660</t>
+          <t>https://openalex.org/W4238849635</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A multi-dimensional analysis of a learner corpus</t>
+          <t>Introduction</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>A multi-dimensional analysis of a learner corpus</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>The present study reports on a multi-dimensional analysis (Biber, 1988) of the Tswana Learner English (TLE) corpus, together with the Louvain Corpus of Native English Essays (LOCNESS). A new multidimensional model is extracted, since the similarities between nativeness and non-nativeness mask differences between linguistic features to such an extent that it is not possible to come to a complete understanding of such differences using the standard 1988 model. A basic five factor model was extracted. Dimension 1 can be taken to capture advanced literacy, specifically as far as complex noun phrase structure is concerned, with the function of expressing information densely. Dimension 2 can be regarded as an indication of transparency and Dimension 3 captures a range of informal style features. The features that group together as Dimension 4 represent a style of writing that is more nuanced and precise and as a provisional label, we propose contextualisation of information. Dimension 5 can be regarded as the persuasive dimension in student writing, a feature that has been identified as a very important characteristic by Biber and Grabe (1987), and also in our own study of student writing. The most striking differences between the two corpora are on Dimensions 1 and 4. LOCNESS shows more advanced literacy than the TLE, and also contextualises information more extensively than the TLE. On the other dimensions, both corpora contain essays that display the various different styles available, showing that as a register, student writing allows for some internal stylistic variation independent of whether the writers are native or non-native speakers of English. The results confirm the usefulness of the multidimensional model, particularly to the extent that a new model is extracted. Substantial overlap between some of the dimensions in this study and dimensions in other models indicate that multidimensional modals are sensitive to particular kinds of feature groupings, which should be taken as evidence in favour of the general validity of this kind of approach.</t>
+          <t>Introduction</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2009-01-01</t>
+          <t>2011-01-01</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1072,17 +1077,17 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789042025981_014</t>
+          <t>https://doi.org/10.1163/ej.9789004201293.i-434.7</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>xiii</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>254</t>
+          <t>xxii</t>
         </is>
       </c>
       <c r="S7" t="b">
@@ -1099,25 +1104,20 @@
       <c r="W7" t="b">
         <v>0</v>
       </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
       <c r="Z7">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AB7">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W955020660</t>
+          <t>https://api.openalex.org/works?filter=cites:W4238849635</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789042025981_014</t>
+          <t>https://doi.org/10.1163/ej.9789004201293.i-434.7</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
@@ -1135,22 +1135,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4387961581</t>
+          <t>https://openalex.org/W3015901506</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Studying Fossil Horses</t>
+          <t>The Difference between Emergency Remote Teaching and Online Learning</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Studying Fossil Horses</t>
+          <t>The Difference between Emergency Remote Teaching and Online Learning</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1988-01-01</t>
+          <t>2024-09-25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1170,42 +1170,62 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004675629</t>
+          <t>https://doi.org/10.1163/9789004702813_021</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>511</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>522</t>
         </is>
       </c>
       <c r="S8" t="b">
         <v>0</v>
       </c>
       <c r="T8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>https://vtechworks.lib.vt.edu/bitstream/10919/104648/1/facdev-article.pdf</t>
         </is>
       </c>
       <c r="W8" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
       </c>
       <c r="Z8">
-        <v>56</v>
+        <v>4254</v>
       </c>
       <c r="AB8">
-        <v>1988</v>
+        <v>2024</v>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4387961581</t>
+          <t>https://api.openalex.org/works?filter=cites:W3015901506</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004675629</t>
+          <t>https://doi.org/10.1163/9789004702813_021</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI8" t="b">
@@ -1218,37 +1238,37 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4242001917</t>
+          <t>https://openalex.org/W2499975532</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Urban Governance in Africa: An Overview</t>
+          <t>The Transformation of Economic Life under the Roman Empire</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Urban Governance in Africa: An Overview</t>
+          <t>The Transformation of Economic Life under the Roman Empire</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Africa is urbanising rapidly and is facing enormous urban challenges, such as the growth of slums and increasing inequality. Secondary cities, with their smaller economies and less capacitated local governments compared to primary cities, face particularly severe challenges. However, responsibility for key urban governance issues is often fragmented amongst large numbers of government stakeholders with limited capacities and conflicting interests. Key urban governance stakeholders therefore need to be brought together in collaborative processes to jointly develop and implement new strategies that are based on a broader range of interests and meet a broader range of needs. In order to be able to do this, understanding actual urban governance processes, which are essentially about how different actors interact to make and operationalise decisions, is vitally important. This chapter highlights the diversity of actors involved in urban governance in Africa and the complexity of urban governance processes, with Kisumu, a secondary city in Kenya, used as an example. Key actors in urban governance in African cities include all levels of government, political parties, traditional leaders, private sector organisations and informal business organisations (such as traders' organisations), international agencies and civil society organisations. The basic objects of urban governance can include a wide range of issues, such as land use management, the provision of basic services, ensuring access/mobility and ensuring public health and safety. The diversity of governance actors and of agendas complicates addressing urban issues, but can also be seen as an opportunity for leveraging additional skills and resources through collaborative urban governance processes that bring different stakeholders together to develop and implement more holistic and inclusive strategies.</t>
+          <t>Did a Roman imperial economy exist under the Late Republic, the Roman Principate and the Later Roman Empire? And if so, what type of economy was it? Another equally important question is: did the Roman Empire, by specific actions, the creation of infrastructures, or its very existence, trigger a transformation of economic life in the regions which it dominated? Or was the Empire a marginal affair in the regions that belonged to it, and did economic developments take their own course, independently of the Empire? Questions like these, which are of great consequence to any student of Roman history, archaeology, and Roman law, are treated in this volume, which in its successive parts focuses on: 1. The character of the Roman economy. 2. Economic life in particular regions of the Roman Empire. 3. The economy of the Later Roman Empire.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2018-10-09</t>
+          <t>2002-01-01</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Brill | Nijhoff eBooks</t>
+          <t>BRILL eBooks</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462967</t>
+          <t>https://openalex.org/S4306462964</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1258,12 +1278,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004387942_004</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>https://brill.com/downloadpdf/book/edcoll/9789004387942/BP000005.pdf</t>
+          <t>https://doi.org/10.1163/9789004401624</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1274,16 +1289,6 @@
       <c r="N9" t="inlineStr">
         <is>
           <t>publishedVersion</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>77</t>
         </is>
       </c>
       <c r="S9" t="b">
@@ -1299,7 +1304,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>https://brill.com/downloadpdf/book/edcoll/9789004387942/BP000005.pdf</t>
+          <t>https://doi.org/10.1163/9789004401624</t>
         </is>
       </c>
       <c r="W9" t="b">
@@ -1311,24 +1316,24 @@
         </is>
       </c>
       <c r="Z9">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="AB9">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4242001917</t>
+          <t>https://api.openalex.org/works?filter=cites:W2499975532</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004387942_004</t>
+          <t>https://doi.org/10.1163/9789004401624</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>book-chapter</t>
+          <t>book</t>
         </is>
       </c>
       <c r="AI9" t="b">
@@ -1341,37 +1346,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2898251808</t>
+          <t>https://openalex.org/W3119037430</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>African Cities and the Development Conundrum</t>
+          <t>Conceptual Domains, Competence, and Chaîne Opératoire in the Levantine Mousterian</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>African Cities and the Development Conundrum</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>This 10th thematic volume of International Development Policy presents a collection of articles exploring some of the complex development challenges associated with Africa’s recent but extremely rapid pace of urbanisation that challenges still predominant but misleading images of Africa as a rural continent. Analysing urban settings through the diverse experiences and perspectives of inhabitants and stakeholders in cities across the continent, the authors consider the evolution of international development policy responses amidst the unique historical, social, economic and political contexts of Africa’s urban development. Contributors include: Carole Ammann, Claudia Baez Camargo, Claire Bénit-Gbaffou, Karen Büscher, Aba Obrumah Crentsil, Sascha Delz, Ton Dietz, Till Förster, Lucy Koechlin, Lalli Metsola, Garth Myers, George Owusu, Edgar Pieterse, Sebastian Prothmann, Warren Smit, and Florian Stoll.</t>
+          <t>Conceptual Domains, Competence, and Chaîne Opératoire in the Levantine Mousterian</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2018-10-16</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Brill | Nijhoff eBooks</t>
+          <t>BRILL eBooks</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462967</t>
+          <t>https://openalex.org/S4306462964</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1381,37 +1381,32 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004387942</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>cc-by-nc</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>publishedVersion</t>
+          <t>https://doi.org/10.1163/9789004369801_027</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>238</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>254</t>
         </is>
       </c>
       <c r="S10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>hybrid</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1163/9789004387942</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="W10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X10" t="inlineStr">
         <is>
@@ -1419,24 +1414,24 @@
         </is>
       </c>
       <c r="Z10">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="AB10">
-        <v>2018</v>
+        <v>2000</v>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2898251808</t>
+          <t>https://api.openalex.org/works?filter=cites:W3119037430</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004387942</t>
+          <t>https://doi.org/10.1163/9789004369801_027</t>
         </is>
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI10" t="b">
@@ -1449,22 +1444,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4249676120</t>
+          <t>https://openalex.org/W2938304724</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Intersectionality</t>
+          <t>‘Grief is love’: Understanding Grief through Self-help Groups Organised by the Family Survivors of Suicide</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Intersectionality</t>
+          <t>‘Grief is love’: Understanding Grief through Self-help Groups Organised by the Family Survivors of Suicide</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>In 2006, the Japanese Government implemented the Basic Act on Suicide Countermeasures in response to an extremely high suicide rate. In accordance with this act, and supported by local government grants, mental health professionals have established support groups in many cities for the family survivors of suicide. Such families have met others like themselves in the support groups and have organised themselves into self-help groups because they were dissatisfied with the concepts of grief work that form the foundation of the professional support. They also felt the need to create new, alternative values and meanings for their grief. This ethnographic research aims to discuss the self-help groups' beliefs regarding grief and the strong cultural influence of Japanese Buddhism on their attitudes toward death and the deceased. The groups' beliefs, which they have developed themselves, and which differ significantly from those of professionals who customarily provide support group services, are examined as 'liberating meaning perspectives'. The three themes identified as perspectives are 'Living with Grief', 'Grief is Ours', and 'Grief is Love'. I also examine how these perspectives influence the social actions of the self-help groups.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2020-11-28</t>
+          <t>2013-01-01</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -1484,17 +1484,17 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004444836_041</t>
+          <t>https://doi.org/10.1163/9781848881235_009</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>310</t>
+          <t>75</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>86</t>
         </is>
       </c>
       <c r="S11" t="b">
@@ -1517,19 +1517,19 @@
         </is>
       </c>
       <c r="Z11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AB11">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4249676120</t>
+          <t>https://api.openalex.org/works?filter=cites:W2938304724</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004444836_041</t>
+          <t>https://doi.org/10.1163/9781848881235_009</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
@@ -1547,37 +1547,37 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://openalex.org/W829779515</t>
+          <t>https://openalex.org/W2970231543</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The Variety Of Housewives And Cockroaches: Examining Code-Choice In Advertisements In Egypt</t>
+          <t>Wilhelm von Humboldt Schriften zur Anthropologie der Basken</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>The Variety Of Housewives And Cockroaches: Examining Code-Choice In Advertisements In Egypt</t>
+          <t>Wilhelm von Humboldt Schriften zur Anthropologie der Basken</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>This chapter examines the discourse function of code-choice in advertisements in Egypt and shows how advertisements reflect and influence attitudes towards language use in the Egyptian community. It defines diglossia and shed light on Badawis levels and their significance for the chapter and shows how the makers of advertisements use code choice and stylistic devices in Egypt with examples from the authors data. The chapter discusses that how code-choice is related to the nature of the product advertised and the target audience. It is divided into two parts, one that deals with sociolinguistic stereotypes specific to Egypt and the second deals with stylistic devices. The cockroach uses ECA negation with the ECA participle form ʾana mis sāmim. So, is Egyptian Colloquial Arabic (ECA) the variety of housewives and cockroaches? Fortunately for us, the answer to this question is no. Keywords: Badawi; cockroaches; code-choice; diglossia; Egyptian Colloquial Arabic (ECA); housewives; sociolinguistic stereotypes; stylistic devices</t>
+          <t>Das Baskenwerk nimmt in der Entwicklung von Humboldts Sprachwissenschaft einen besonderen Stellenwert ein. Baskisch ist die erste nicht-indogermanische Sprache, mit der er sich wissenschaftlich beschäftigte, und die einzige, deren Land er bereiste. Intensiv hat er sich auch mit der autochthonen baskischen Sprachwissenschaft auseinandergesetzt und wurde von ihr stark beeinflusst, was im deutschen Sprachraum nur wenig bekannt ist. Die zweite Abteilung der Edition von Humboldts sprachwissenschaftlichen Schriften versucht, Humboldts ursprünglichen Plan seines bisher nur zum Teil veröffentlichten Baskenwerks nachzuzeichnen. Der Ansatz, den Humboldt in seinen baskischen Schriften verfolgt, erschöpft sich nicht in einer Annäherung an die baskische Sprache (Band 2 und 3 der Abteilung); vielmehr kristallisiert sich sehr klar der anthropologische Zugang heraus. In den hier veröffentlichten Schriften des ersten Bandes der Abteilung, für die Humboldt die Form der Reisebeschreibungen wählt, äußert er sich zum Land, zu den Menschen, Lebensformen und Traditionen, zur sozialen Organisation und zur Geschichte der Basken.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2009-01-01</t>
+          <t>2010-01-01</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>BRILL eBooks</t>
+          <t>Brill | Schöningh eBooks</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462964</t>
+          <t>https://openalex.org/S4306462969</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1587,17 +1587,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004172128.i-298.109</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>271</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>284</t>
+          <t>https://doi.org/10.30965/9783657767342</t>
         </is>
       </c>
       <c r="S12" t="b">
@@ -1616,28 +1606,28 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>en</t>
+          <t>de</t>
         </is>
       </c>
       <c r="Z12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AB12">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W829779515</t>
+          <t>https://api.openalex.org/works?filter=cites:W2970231543</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004172128.i-298.109</t>
+          <t>https://doi.org/10.30965/9783657767342</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>book-chapter</t>
+          <t>book</t>
         </is>
       </c>
       <c r="AI12" t="b">
@@ -1650,27 +1640,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3045246892</t>
+          <t>https://openalex.org/W2275083532</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The seven deadly sins : from communities to individuals</t>
+          <t>Local Economies? Production and Exchange of Inland Regions in Late Antiquity</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The seven deadly sins : from communities to individuals</t>
+          <t>Local Economies? Production and Exchange of Inland Regions in Late Antiquity</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>List of Illustrations Acknowledgments List of Contributors Introduction: Cultural Construction and the Vices, Richard Newhauser I. COMMUNITIES 1. Sin and the Construction of Carolingian Kingship, Dwight D. Allman 2. Envy in the Intellectual Discourse of the High Middle Ages, Bridget K. Balint 3. 'The Ooze of Gluttony': Attitudes towards Food, Eating, and Excess in the Middle Ages, Susan E. Hill II. THE INSTITUTION OF THE CHURCH 4. Cassian, Nocturnal Emissions, and the Sexuality of Jesus, John Kitchen 5. Pride Goes Before a Fall: Aldhelm's Practical Application of Gregorian and Cassianic Conceptions of Superbia and the Eight Principal Vices, Rhonda L. McDaniel 6. Biblical Liars and Thirteenth-Century Theologians, Dallas G. Denery II 7. 'The Hard Bed of the Cross': Good Friday Preaching and the Seven Deadly Sins, Holly Johnson 8. Dressed to the Sevens, or Sin in Style: Fashion Statements by the Deadly Vices in Spanish Baroque Autos Sacramentales, Hilaire Kallendorf III. INDIVIDUALS 9. 'Blessed are they that hunger after justice': From Vice to Beatitude in Dante's Purgatorio, V. S. Benfell III 10. Greed and Anti-Fraternalism in Chaucer's 'Summoner's Tale', Derrick G. Pitard 11. Social Status and Sin: Reading Bosch's Prado Seven Deadly Sins and Four Last Things Painting, Laura D. Gelfand 12. Freud as Virgil: The Anthropologies of Psychoanalysis and the Commedia, Thomas Parisi Bibliography Indices</t>
+          <t>Acknowledgements -- List of contributors -- Local economies in late antiquity? : some thoughts / Luke Lavan -- The late antique economy : approaches, methods and conceptual issues / Alyssa A. Bandow -- The late antique economy : regional surveys / Andrea Zerbini -- The late antique economy : primary and secondary production / Andrea Zerbini -- The late antique economy : infrastructures of transport and retail / Alyssa A. Bandow -- The late antique economy : ceramics and trade / Stefano Costa -- A comparative perspective on the late antique economy / Mark Whittow -- Integration and disintegration in the late Roman economy : the role of markets, emperors, and aristocrats / Peter Sarris -- Production in inland regions -- Villas, taxes and trade in fourth century hispania / Kim Bowes -- The lessons of Gaulish sigillata and other finewares / Tamara Lewit -- Patterning the late antique economies of inland sicily in a Mediterranean context / Emanuele Vaccaro -- Diana Veteranorum and the dynamics of an inland economy / Elizabeth Fentress -- The economic expansion of the anatolian countryside in late antiquity : the coast versus inland regions / Adam Izdebski -- The urban economy in southern inland greater Syria from the seventh century to the end of the umayyads / Fanny Bessard -- Exchange in inland regions -- Balancing the scales : Romano-British pottery in early late antiquity / Jeremy Evans -- The supply and distribution of ceramic building material in Roman Britain / Phil Mills -- Imported and local pottery in late Roman Pannonia / Piroska Harshegyi and Katalin Ottomanyi -- Africa : patterns of consumption in coastal regions versus inland regions : the ceramic evidence (300-700 a.d.) / Michel Bonifay -- Pottery production and exchange in late antique syria (fourth-eighth century A.D.). a study of some imported and local wares / Agnes Vokaer -- Abstracts in French -- Indices -- Themes -- Index of places.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2007-01-01</t>
+          <t>2015-02-01</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1690,7 +1680,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>https://ci.nii.ac.jp/ncid/BA81711596</t>
+          <t>https://kar.kent.ac.uk/48371/</t>
         </is>
       </c>
       <c r="S13" t="b">
@@ -1713,14 +1703,14 @@
         </is>
       </c>
       <c r="Z13">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="AB13">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W3045246892</t>
+          <t>https://api.openalex.org/works?filter=cites:W2275083532</t>
         </is>
       </c>
       <c r="AF13" t="inlineStr">
@@ -1738,27 +1728,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2152428980</t>
+          <t>https://openalex.org/W4388645775</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Encyclopedia of Arabic Language and Linguistics</t>
+          <t>Some Remarks on Fortified Settlements in The Attic Countryside</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Encyclopedia of Arabic Language and Linguistics</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>This volume concludes the publication of the Encyclopedia of Arabic Language and Linguistics in print. It represents a unique collaboration of over hundreds of scholars from around the world, covering all relevant aspects of the study of Arabic and dealing with all levels of the language (pre-Classical Arabic, Classical Arabic, Modern Standard Arabic, Arabic vernaculars, mixed varieties of Arabic). No other reference work offers this scale of contributions or depth and breadth of coverage. The Encyclopedia of Arabic Language and Linguistics is, therefore, a standard reference work for students and researchers in the field of linguistics, Islamic studies, Arabic literature and other related fields.</t>
+          <t>Some Remarks on Fortified Settlements in The Attic Countryside</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2006-01-01</t>
+          <t>1992-01-01</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1778,7 +1763,17 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>http://repository.ubn.ru.nl/handle/2066/41297</t>
+          <t>https://doi.org/10.1163/9789004673298_010</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>91</t>
         </is>
       </c>
       <c r="S14" t="b">
@@ -1801,19 +1796,24 @@
         </is>
       </c>
       <c r="Z14">
-        <v>322</v>
+        <v>28</v>
       </c>
       <c r="AB14">
-        <v>2006</v>
+        <v>1992</v>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2152428980</t>
+          <t>https://api.openalex.org/works?filter=cites:W4388645775</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004673298_010</t>
         </is>
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI14" t="b">
@@ -1826,37 +1826,37 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://openalex.org/W368225393</t>
+          <t>https://openalex.org/W2740713369</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Agency and Causation in the Human Sciences</t>
+          <t>Research in the Social Scientific Study of Religion</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Agency and Causation in the Human Sciences</t>
+          <t>Research in the Social Scientific Study of Religion</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>In everyday life, we explain and predict human actions through beliefs and intentions. We also assume the existence of persons who act on the basis of reasons. Naturalist philosophers do not accept this concept of 'agent causality': what common sense and sociological explanations called reasons should be interpreted as normal causes of actions. As a matter of fact social sciences increasingly use the causal model of the natural sciences in order to explain human actions. In this volume leading specialists in action theory discuss the question: Is the causal model of the natural sciences sufficient to explain human actions or can we expect an explanatory advantage from the classical concept of agent causality? Contributors: R. Boudon, F. Castellani, A. Corradini, M. De Caro, S. Galvan, G. Keil, E. J. Lowe, U. Meixner, A. Mele, T. O'Connor, J. Quitterer, E. Runggaldier, A. Varzi, H. Weidemann</t>
+          <t>This volume includes a wide range of papers that explore individual and institutional aspects of religion from a social-science perspective. The special section has articles related to the practice of prayer, and includes studies from the USA, Europe, and the Middle East. The general papers include studies on coping strategies, God representations, spirituality versus religion, self-control in a Muslim context, and faith-based organizations in Cambodia. Together these papers form a valuable collection indicating the depth and vibrancy of research in these fields.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2007-01-01</t>
+          <t>1999-01-01</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Brill | mentis eBooks</t>
+          <t>BRILL eBooks</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306486262</t>
+          <t>https://openalex.org/S4306462964</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1866,7 +1866,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>https://doi.org/10.30965/9783969750469</t>
+          <t>https://doi.org/10.1163/9789004496231_019</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>281</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>281</t>
         </is>
       </c>
       <c r="S15" t="b">
@@ -1889,24 +1899,24 @@
         </is>
       </c>
       <c r="Z15">
-        <v>18</v>
+        <v>463</v>
       </c>
       <c r="AB15">
-        <v>2007</v>
+        <v>1999</v>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W368225393</t>
+          <t>https://api.openalex.org/works?filter=cites:W2740713369</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>https://doi.org/10.30965/9783969750469</t>
+          <t>https://doi.org/10.1163/9789004496231_019</t>
         </is>
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI15" t="b">
@@ -1919,27 +1929,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://openalex.org/W582357572</t>
+          <t>https://openalex.org/W624160020</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Handbook of the Syllable</t>
+          <t>Development and Decline of Fukien Province in the 17th and 18th Centuries</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Handbook of the Syllable</t>
+          <t>Development and Decline of Fukien Province in the 17th and 18th Centuries</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>The Handbook of the Syllable approaches the study of the phonology and phonetics of the syllable with theoretical, empirical and methodological heterogeneity as its guiding principle. Since the mid-nineteenth century, scholars in the phonetic and phonological sciences have found it convenient to refer to the syllable, but definitions are scarce and none apply to all areas where the syllable is frequently invoked. The Handbook’s seventeen chapters focus on empirical studies of the syllable by presenting both new data and new kinds of data. The work addresses the syllable in phonology, phonetics, experimental psycholinguistics, neurolinguistics, diachronic linguistics, and orthography. It is a seminal reference book for researchers exploring any empirical area where the notion of 'the syllable' is invoked.</t>
+          <t>The history of China's Southeast coast has unusual features. For many centuries, overseas trade and migration, internal and external warfare, strong religious beliefs and receptiveness to foreign influences characterized this society of fiercely independent traders, fishermen and mountain farmers. The protracted struggle of Cheng Ch'eng- kung and the Southern Ming against the Ch'ing dynasty precipitated Fukien into a crisis, from which many chose to escape by emigration to the Philippines and Taiwan. Recovery was slow. ; The fourteen Western and Chinese contributors to this study focus on internal economic and social developments, overseas and religious change. From the rich Chinese and European source materials, a picture emerges of great regional diversity. Local interests and values were confronted by the central government's orthodox rule, and Western influences of Jesuits and traders. The Fukienese reaction to them produces fascinating insights into Chinese society, and a truly local history which may qualify our ideas on the Chinese Empire. REA sinologists, social and economic historians.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2011-01-01</t>
+          <t>1990-01-01</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1959,7 +1969,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004187405.i-464</t>
+          <t>https://doi.org/10.1163/9789004488458</t>
         </is>
       </c>
       <c r="S16" t="b">
@@ -1982,19 +1992,19 @@
         </is>
       </c>
       <c r="Z16">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="AB16">
-        <v>2011</v>
+        <v>1990</v>
       </c>
       <c r="AC16" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W582357572</t>
+          <t>https://api.openalex.org/works?filter=cites:W624160020</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004187405.i-464</t>
+          <t>https://doi.org/10.1163/9789004488458</t>
         </is>
       </c>
       <c r="AF16" t="inlineStr">
@@ -2012,27 +2022,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://openalex.org/W851674540</t>
+          <t>https://openalex.org/W4292838531</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Chapter Five. The Syllable As Delimitation Of The Base For Reduplication</t>
+          <t>Indonesian Higher Education during the COVID-19 Pandemic</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chapter Five. The Syllable As Delimitation Of The Base For Reduplication</t>
+          <t>Indonesian Higher Education during the COVID-19 Pandemic</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>This chapter demonstrates that access to the prosodic category of the syllable is crucial for certain morphological processes in some languages. Specifically, it shows that the syllable can serve as delimitation on the base for copying in reduplication. This, coupled with other morphologically based evidence, indicates that the syllable must be a legitimate constituent in phonology, and one that must be accessible by the morphology. The chapter discusses the notion of delimiting a subset of a given stem as the base for reduplication, and it also discusses such base-delimitation in the context of the typologically unusual pattern of 'syllable copy' reduplication. The chapter presents definitive example of the syllable serving as the base for reduplication. It outlines the aforementioned opacity in base-assignment from Hiaki. The chapter reviews the concept of base delimitation in theoretical approaches that do not utilize 'phonological copying'. Keywords: morphology; phonology; reduplication; syllable</t>
+          <t>At the onset of the COVID-19 pandemic, Indonesia announced major higher education (HE) policies called Kampus Merdeka and launched the Mid-Term National Development Plan and the Strategic Plan of the Ministry of Education and Culture. While none of these policies anticipated the pandemic, two aspects of the policies have been somewhat accelerated by the pandemic, though not without problems. These are: greater autonomy for state HE institutions and proliferation of distance/online education. The pandemic provides a greater autonomy for most state HE institutions to manage their education services. However, they are increasingly drawn into the governments’ public health campaigns, exerting their facilities and human resources. Seemingly, the autonomy of HE institutions has to be in compliance with government agendas. While HE institutions throughout the archipelago instantly shifted into online learning due to the pandemic, to what degree online learning can be a permanent feature of Indonesian HE is still questionable. The chapter ends with an examination of the possible landscape of the Indonesian HE sector post-COVID-19 and the remaining challenges.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2011-01-01</t>
+          <t>2022-06-02</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2052,17 +2062,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004187405.i-464.38</t>
+          <t>https://doi.org/10.1163/9789004520554_016</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>129</t>
+          <t>262</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>279</t>
         </is>
       </c>
       <c r="S17" t="b">
@@ -2085,19 +2095,19 @@
         </is>
       </c>
       <c r="Z17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AB17">
-        <v>2011</v>
+        <v>2022</v>
       </c>
       <c r="AC17" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W851674540</t>
+          <t>https://api.openalex.org/works?filter=cites:W4292838531</t>
         </is>
       </c>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004187405.i-464.38</t>
+          <t>https://doi.org/10.1163/9789004520554_016</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr">
@@ -2115,37 +2125,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://openalex.org/W879504256</t>
+          <t>https://openalex.org/W2061443247</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wadi Hammeh 27, an Early Natufian Settlement at Pella in Jordan</t>
+          <t>On law and policy in the European Court of Justice : a comparative study in judicial policymaking</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Wadi Hammeh 27, an Early Natufian Settlement at Pella in Jordan</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Winner of the 2013 American Schools of Oriental Research G. Ernest Wright Award! This award is given to the most substantial volume dealing with archaeological material, excavation reports and material culture from the ancient Near East and eastern Mediterranean.Wadi Hammeh 27, an Early Natufian Settlement at Pella in Jordan is a detailed report on one of the most important Natufian sites to have emerged in the past thirty years and an integrated analysis and interpretation of subsistence strategies, settlement patterns and ritual life in one of the world’s earliest village communities. The 14,000-year-old settlement of Wadi Hammeh 27 is one of the most spectacular sites of its kind, featuring the largest, most complex pre-Neolithic architectural complex yet discovered in the Middle East, an unparalleled series of artefact caches and activity areas, and a rich corpus of late Ice Age art pieces. "This book is a treasure-trove for researchers specialising in the Natufian period and is a most significant addition to the data base of the Early Natufian in particular." Anna Belfer-Cohen, Hebrew University of Jerusalem</t>
+          <t>On law and policy in the European Court of Justice : a comparative study in judicial policymaking</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2013-01-01</t>
+          <t>1986-06-01</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>BRILL eBooks</t>
+          <t>Brill | Nijhoff eBooks</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462964</t>
+          <t>https://openalex.org/S4306462967</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2155,27 +2160,22 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004236103</t>
+          <t>https://brill.com/view/title/9727</t>
         </is>
       </c>
       <c r="S18" t="b">
         <v>0</v>
       </c>
       <c r="T18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="V18" t="inlineStr">
-        <is>
-          <t>http://swbplus.bsz-bw.de/bsz376292210kla.htm</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="W18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X18" t="inlineStr">
         <is>
@@ -2183,19 +2183,14 @@
         </is>
       </c>
       <c r="Z18">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="AB18">
-        <v>2013</v>
+        <v>1986</v>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W879504256</t>
-        </is>
-      </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1163/9789004236103</t>
+          <t>https://api.openalex.org/works?filter=cites:W2061443247</t>
         </is>
       </c>
       <c r="AF18" t="inlineStr">
@@ -2213,27 +2208,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4229899453</t>
+          <t>https://openalex.org/W3134656133</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Excavations at Tall Jawa, Jordan</t>
+          <t>From ‘False’ to ‘Reified’ Consciousness: Tracing the isr’s Critical Research on Authoritarianism</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Excavations at Tall Jawa, Jordan</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>In Excavations at Tall Jawa, Jordan, Volume 5, the authors present their research in the areas of regional survey, salvage excavation, zooarchaeology, ceramic typology, experimental archaeology and ethnoarchaeology. This work illustrates areas threatened and later destroyed by modern development and is a contribution to heritage documentation. These studies illuminate aspects of family and town life in the Iron Age, Roman, Byzantine and Late Ottoman–Early Mandate periods in central Jordan.</t>
+          <t>From ‘False’ to ‘Reified’ Consciousness: Tracing the isr’s Critical Research on Authoritarianism</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2016-08-01</t>
+          <t>2021-02-09</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -2253,18 +2243,43 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004316201</t>
+          <t>https://doi.org/10.1163/9789004444744_013</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>cc-by</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>publishedVersion</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>347</t>
         </is>
       </c>
       <c r="S19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004444744_013</t>
         </is>
       </c>
       <c r="W19" t="b">
@@ -2276,24 +2291,24 @@
         </is>
       </c>
       <c r="Z19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB19">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="AC19" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4229899453</t>
+          <t>https://api.openalex.org/works?filter=cites:W3134656133</t>
         </is>
       </c>
       <c r="AE19" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004316201</t>
+          <t>https://doi.org/10.1163/9789004444744_013</t>
         </is>
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI19" t="b">
@@ -2306,22 +2321,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4388679467</t>
+          <t>https://openalex.org/W3162444750</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ammonite Territory and Sites</t>
+          <t>Siegfried Kracauer and the Interpretation of Films</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Ammonite Territory and Sites</t>
+          <t>Siegfried Kracauer and the Interpretation of Films</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1999-01-01</t>
+          <t>2021-02-09</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -2341,28 +2356,43 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004667884_004</t>
+          <t>https://doi.org/10.1163/9789004444744_016</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>cc-by</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>publishedVersion</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>391</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>411</t>
         </is>
       </c>
       <c r="S20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>hybrid</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004444744_016</t>
         </is>
       </c>
       <c r="W20" t="b">
@@ -2377,16 +2407,16 @@
         <v>2</v>
       </c>
       <c r="AB20">
-        <v>1999</v>
+        <v>2021</v>
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4388679467</t>
+          <t>https://api.openalex.org/works?filter=cites:W3162444750</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004667884_004</t>
+          <t>https://doi.org/10.1163/9789004444744_016</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
@@ -2404,27 +2434,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4249731245</t>
+          <t>https://openalex.org/W90963207</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Boethius in the Middle Ages</t>
+          <t>The British Army in North America and the West Indies, 1755–83: A Medical Perspective</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Boethius in the Middle Ages</t>
+          <t>The British Army in North America and the West Indies, 1755–83: A Medical Perspective</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Boethius' Consolatio Philosophiae is one of those exceptional works that circulated widely throughout such diverse medieval cultures as the schools and universities, the court, and religious houses. It spawned a rich tradition of Latin commentaries and was a major force in shaping vernacular literary traditions, including the works of Jean de Meun, Dante, and Chaucer. The changing perceptions of the Consolatio are the subject of this collection of new essays. The first section is devoted to the Latin commentary tradition (William of Conches, Nicholas Trevet, and Pierre d'Ailly). The other sections explore the vernacular traditions (Italian, French, German, English, and Dutch). The book underlines the interactions between the Latin and the vernacular and between literary and scholastic contexts, and the focus throughout is on the intellectual and institutional background of the works discussed.</t>
+          <t>This chapter provides an analytical overview of the operational structure, hospital and regimental systems of military medical practice of the British Army in North Amercia and the West Indies, 1755-83, using a database of medical officers, regimental returns, lists of drugs used, correspondence and publications. Practice varied depending on location, season, and time of year, but cooperation between medical and general officers was crucial. Pringle's emphasis on environment influenced practice, with medics advocating preventative treatments. Army practitioners were among medical officers in the West Indies, at the forefront of moderate therapeutics.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1997-01-01</t>
+          <t>2007-01-01</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -2444,7 +2474,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004452121</t>
+          <t>https://doi.org/10.1163/9789401204934_007</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>86</t>
         </is>
       </c>
       <c r="S21" t="b">
@@ -2467,24 +2507,24 @@
         </is>
       </c>
       <c r="Z21">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="AB21">
-        <v>1997</v>
+        <v>2007</v>
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4249731245</t>
+          <t>https://api.openalex.org/works?filter=cites:W90963207</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004452121</t>
+          <t>https://doi.org/10.1163/9789401204934_007</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>article</t>
         </is>
       </c>
       <c r="AI21" t="b">
@@ -2497,22 +2537,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2264742718</t>
+          <t>https://openalex.org/W3157694986</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Logic and Conversation</t>
+          <t>Conceptualising a Black Feminist Arts Pedagogy</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Logic and Conversation</t>
+          <t>Conceptualising a Black Feminist Arts Pedagogy</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1975-12-12</t>
+          <t>2020-09-30</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -2532,17 +2572,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004368811_003</t>
+          <t>https://doi.org/10.1163/9789004442870_024</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>242</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>251</t>
         </is>
       </c>
       <c r="S22" t="b">
@@ -2565,19 +2605,19 @@
         </is>
       </c>
       <c r="Z22">
-        <v>19875</v>
+        <v>1</v>
       </c>
       <c r="AB22">
-        <v>1975</v>
+        <v>2020</v>
       </c>
       <c r="AC22" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2264742718</t>
+          <t>https://api.openalex.org/works?filter=cites:W3157694986</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004368811_003</t>
+          <t>https://doi.org/10.1163/9789004442870_024</t>
         </is>
       </c>
       <c r="AF22" t="inlineStr">
@@ -2595,32 +2635,32 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4402753148</t>
+          <t>https://openalex.org/W1533383006</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Posyandu</t>
+          <t>20 Introduction of an Appellate Review Mechanism for International Investment Disputes: Expected Benefits and Remaining Tasks</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Posyandu</t>
+          <t>20 Introduction of an Appellate Review Mechanism for International Investment Disputes: Expected Benefits and Remaining Tasks</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1996-01-01</t>
+          <t>2015-01-01</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>BRILL eBooks</t>
+          <t>Brill | Nijhoff eBooks</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462964</t>
+          <t>https://openalex.org/S4306462967</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2630,17 +2670,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004643123_008</t>
+          <t>https://doi.org/10.1163/9789004291102_022</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>474</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>495</t>
         </is>
       </c>
       <c r="S23" t="b">
@@ -2657,20 +2697,25 @@
       <c r="W23" t="b">
         <v>0</v>
       </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
       <c r="Z23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AB23">
-        <v>1996</v>
+        <v>2015</v>
       </c>
       <c r="AC23" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4402753148</t>
+          <t>https://api.openalex.org/works?filter=cites:W1533383006</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004643123_008</t>
+          <t>https://doi.org/10.1163/9789004291102_022</t>
         </is>
       </c>
       <c r="AF23" t="inlineStr">
@@ -2688,27 +2733,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3114973174</t>
+          <t>https://openalex.org/W4250529825</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>MOOCs, Students, Higher Education and Their Paradoxes</t>
+          <t>Keeping Your Ear to the Cosmos: Coherence as the Standard of Good Music in the Northern Song</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MOOCs, Students, Higher Education and Their Paradoxes</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Massive Open Online Courses (moocs) have attracted a great deal of attention in the media. Some of this coverage has promoted myths to the effect that moocs are completely new (not a continuation of previous practices in education), monolithic, and inevitable. They are not. The author provides an extensive discussion of how moocs have developed from previous practices of distance education, lifelong learning, and open educational resources. She then explains why moocs are "fragile," mainly because they are in clear danger of not living up to the hype that has surrounded them. And they are not monolithic: various types have emerged, and more continue to emerge. The author concludes with the observation that the mooc movement is one of many "wicked paradoxes" that will be very challenging for higher educational institutions to address.</t>
+          <t>Keeping Your Ear to the Cosmos: Coherence as the Standard of Good Music in the Northern Song</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2019-02-25</t>
+          <t>2020-02-20</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -2728,17 +2768,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004393073_009</t>
+          <t>https://doi.org/10.1163/9789004423626_008</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>277</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>309</t>
         </is>
       </c>
       <c r="S24" t="b">
@@ -2761,19 +2801,19 @@
         </is>
       </c>
       <c r="Z24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB24">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="AC24" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W3114973174</t>
+          <t>https://api.openalex.org/works?filter=cites:W4250529825</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004393073_009</t>
+          <t>https://doi.org/10.1163/9789004423626_008</t>
         </is>
       </c>
       <c r="AF24" t="inlineStr">
@@ -2791,22 +2831,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://openalex.org/W799501272</t>
+          <t>https://openalex.org/W4236552060</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Differential Object Marking in the First Original Romanian Texts</t>
+          <t>Commentary on “Inquiry, Activity and Epistemic Practice”</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Differential Object Marking in the First Original Romanian Texts</t>
+          <t>Commentary on “Inquiry, Activity and Epistemic Practice”</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2015-01-01</t>
+          <t>2008-01-01</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2826,17 +2866,17 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004292550_007</t>
+          <t>https://doi.org/10.1163/9789460911453_010</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>118</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>245</t>
+          <t>122</t>
         </is>
       </c>
       <c r="S25" t="b">
@@ -2859,19 +2899,19 @@
         </is>
       </c>
       <c r="Z25">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AB25">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W799501272</t>
+          <t>https://api.openalex.org/works?filter=cites:W4236552060</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004292550_007</t>
+          <t>https://doi.org/10.1163/9789460911453_010</t>
         </is>
       </c>
       <c r="AF25" t="inlineStr">
@@ -2889,22 +2929,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2918080062</t>
+          <t>https://openalex.org/W167558857</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A Shifting Paradigm in Teaching and Learning</t>
+          <t>Maintenance of biodiversity through predation in freshwater nematodes?</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>A Shifting Paradigm in Teaching and Learning</t>
+          <t>Maintenance of biodiversity through predation in freshwater nematodes?</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>SummaryPrédation is one important factor maintaining species diversity in stable and homogenous habitats. Predators enhance species richness by preventing competitive exclusion, or by physical disturbance. In this study we investigate whether predators increase species richness of freshwater nematodes, the dominant and most specious taxon in benthic food webs. Chironomid larvae and the turbellarian Planada torva preyed on nematodes in Petri dishes, whereas annelids did not affect nematode abundance. In microcosm experiments, these macrobenthic taxa influenced neither total nematode abundance nor species richness. However, they reduced the abundance of the two dominant species. Subdominant species increased, which can lead to small-scale environmental variability. In the field we tested whether predators would increase the number of coexisting nematode species. We found a strong positive correlation between the abundance of predatory nematodes and species number, but no effect of possible macrobenthic predators on nematode diversity could be shown.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2009-01-01</t>
+          <t>2004-01-01</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2924,17 +2969,17 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789087906962_002</t>
+          <t>https://doi.org/10.1163/9789004475236_068</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>723</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>737</t>
         </is>
       </c>
       <c r="S26" t="b">
@@ -2957,19 +3002,19 @@
         </is>
       </c>
       <c r="Z26">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="AB26">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="AC26" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2918080062</t>
+          <t>https://api.openalex.org/works?filter=cites:W167558857</t>
         </is>
       </c>
       <c r="AE26" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789087906962_002</t>
+          <t>https://doi.org/10.1163/9789004475236_068</t>
         </is>
       </c>
       <c r="AF26" t="inlineStr">
@@ -2987,27 +3032,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://openalex.org/W754474959</t>
+          <t>https://openalex.org/W4239035690</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Plato On Akrasia And Knowing Your Own Mind</t>
+          <t>Gender Conflicts, Miscommunication, and Communicative Communities in the Late Middle Ages: The Evidence of Fifteenth-Century German Verse Narratives</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Plato On Akrasia And Knowing Your Own Mind</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>The standard picture of the development of Plato’s views on akrasia depicts an increase in subtlety and psychological realism from the early to the middle and late dialogues. In the Republic , Plato partitions the soul and thus recognizes the existence of non-rational motivations that do not aim at what is best for the whole person overall. Plato’s theory in the Protagoras may be reminiscent of the claim that he makes about desire and the good in the Gorgias and the Meno . The chapter draws on literature on self-knowledge to sketch several worries to which one’s lack of awareness of one’s own mind might give rise. It turns to the details of Plato’s solution to the puzzle of apparent akratic action in the Protagoras . Finally, the chapter concludes with a few brief remarks about what the lines of thought that were explored may suggest about Plato’s conception of rationality. Keywords: akrasia ; Gorgias ; non-rational motivation; Plato; Protagoras ; psychological realism; Republic ; self-knowledge</t>
+          <t>Gender Conflicts, Miscommunication, and Communicative Communities in the Late Middle Ages: The Evidence of Fifteenth-Century German Verse Narratives</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2007-01-01</t>
+          <t>2003-01-01</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3027,17 +3067,17 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004156708.i-308.18</t>
+          <t>https://doi.org/10.1163/9789047401964_007</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>65</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>92</t>
         </is>
       </c>
       <c r="S27" t="b">
@@ -3060,19 +3100,19 @@
         </is>
       </c>
       <c r="Z27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB27">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W754474959</t>
+          <t>https://api.openalex.org/works?filter=cites:W4239035690</t>
         </is>
       </c>
       <c r="AE27" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/ej.9789004156708.i-308.18</t>
+          <t>https://doi.org/10.1163/9789047401964_007</t>
         </is>
       </c>
       <c r="AF27" t="inlineStr">
@@ -3090,32 +3130,37 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4236432387</t>
+          <t>https://openalex.org/W841912214</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>5 Appropriating Genius: Jin Shengtan’s Construction of Textual Authority and Authorship in His Commented Edition of Shuihu Zhuan (The Water Margin Saga)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>5 Appropriating Genius: Jin Shengtan’s Construction of Textual Authority and Authorship in His Commented Edition of Shuihu Zhuan (The Water Margin Saga)</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Jin Shengtan is a great name in traditional Chinese literary criticism. His commentary edition of Shuihu zhuan , which he entitled Di-wu caizi shu Shi Nai'an Shuihu zhuan ( The Fifth Book of Genius: Shi Nai'an's Water Margin Saga , latest preface 1641), stands out as a monument in his critical oeuvre, and in the history of editions of Chinese literature. This chapter suggests that the edited and commented text that he published some twenty-five years later was the result of this early stage of juvenile enthusiasm. Although Jin Shengtan's commented Water Margin edition is considered as a milestone in the history of Chinese fiction publishing and literary criticism, the circumstances of the original production of this edition have remained largely unstudied. As one point on which there is some confusion in modern research on Jin Shengtan, Guanhuatang has long been assumed to have been the studio name of a friend of Jin's. Keywords: Chinese literature; Guanhuatang; Jin Shengtan; juvenile enthusiasm; Shuihu zhuan; traditional Chinese literary criticism</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2012-01-01</t>
+          <t>2014-01-01</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Brill | Nijhoff eBooks</t>
+          <t>BRILL eBooks</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://openalex.org/S4306462967</t>
+          <t>https://openalex.org/S4306462964</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -3125,17 +3170,17 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004218642_014</t>
+          <t>https://doi.org/10.1163/9789004279421_007</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>361</t>
+          <t>163</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>408</t>
+          <t>194</t>
         </is>
       </c>
       <c r="S28" t="b">
@@ -3152,20 +3197,25 @@
       <c r="W28" t="b">
         <v>0</v>
       </c>
+      <c r="X28" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
       <c r="Z28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB28">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="AC28" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4236432387</t>
+          <t>https://api.openalex.org/works?filter=cites:W841912214</t>
         </is>
       </c>
       <c r="AE28" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004218642_014</t>
+          <t>https://doi.org/10.1163/9789004279421_007</t>
         </is>
       </c>
       <c r="AF28" t="inlineStr">
@@ -3183,22 +3233,38 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2171293646</t>
+          <t>https://openalex.org/W3006978447</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Metaphysics in Contemporary Physics</t>
+          <t>Scenario-Based Learning</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Metaphysics in Contemporary Physics</t>
+          <t>Scenario-Based Learning</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Continuing the theme of using the real world as a teaching resource,_x000D_
+Smith, Warnes and van Hoestenberghe describe learning scenarios where_x000D_
+students find their own way and make their own choices in exploring_x000D_
+an authentic situation. The intended learning outcomes are explained to_x000D_
+the students to guide them to what is relevant, but these are thoroughly_x000D_
+embedded in the tasks set: they do not have to make a special effort_x000D_
+to work out what is being assessed. Again, assessment requires careful_x000D_
+thought, which makes having student input to the design all the more_x000D_
+relevant; this allows the teaching staff to actively guide students through_x000D_
+their learning rather than merely acting as dispensers of knowledge: just_x000D_
+as the Connected Curriculum strategy invites, students find things out for_x000D_
+themselves.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2015-11-21</t>
+          <t>2024-12-03</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -3218,7 +3284,17 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004310827</t>
+          <t>https://doi.org/10.1163/9789004719118_071</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>71</t>
         </is>
       </c>
       <c r="S29" t="b">
@@ -3241,24 +3317,24 @@
         </is>
       </c>
       <c r="Z29">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="AB29">
-        <v>2015</v>
+        <v>2024</v>
       </c>
       <c r="AC29" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2171293646</t>
+          <t>https://api.openalex.org/works?filter=cites:W3006978447</t>
         </is>
       </c>
       <c r="AE29" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004310827</t>
+          <t>https://doi.org/10.1163/9789004719118_071</t>
         </is>
       </c>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI29" t="b">
@@ -3271,22 +3347,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2486730578</t>
+          <t>https://openalex.org/W2903940037</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The Mysterious Moment: early Dada performance as ritual</t>
+          <t>Implementing Virtual Reality in the Classroom: Envisaging Possibilities in stem Education</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>The Mysterious Moment: early Dada performance as ritual</t>
+          <t>Implementing Virtual Reality in the Classroom: Envisaging Possibilities in stem Education</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>With the advancement of immersive virtual reality (VR) there are various possibilities with the introduction of these technologies. Preparing students to effectively navigate, contribute to, and participate in virtual environments appears to be an important set of stem-related competencies in the future. This chapter describes the VR Education Model (VEM), describing elements of this technology and its possible application in the classroom. One factor in student underachievement in stem subjects may be a heavy reliance upon textual representations at the expense of more visuo spatial representations. Therefore, the use of VR may be particularly beneficial when representing and learning about stem-related concepts. The authors envisage a number of scenarios that include but are not limited to the possibilities described in this chapter. The implementation of VR is discussed in terms of a broader stem vision that meets the unique needs and priorities of each school.</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2006-01-01</t>
+          <t>2018-10-22</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -3306,17 +3387,17 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789042029545_004</t>
+          <t>https://doi.org/10.1163/9789004391413_005</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>61</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>73</t>
         </is>
       </c>
       <c r="S30" t="b">
@@ -3339,19 +3420,19 @@
         </is>
       </c>
       <c r="Z30">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="AB30">
-        <v>2006</v>
+        <v>2018</v>
       </c>
       <c r="AC30" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2486730578</t>
+          <t>https://api.openalex.org/works?filter=cites:W2903940037</t>
         </is>
       </c>
       <c r="AE30" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789042029545_004</t>
+          <t>https://doi.org/10.1163/9789004391413_005</t>
         </is>
       </c>
       <c r="AF30" t="inlineStr">
@@ -3369,22 +3450,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://openalex.org/W4327515011</t>
+          <t>https://openalex.org/W4381514609</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>English Literary History</t>
+          <t>Queer Joy as an Affective Incitement to Queer and Trans Studies in Education</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>English Literary History</t>
+          <t>Queer Joy as an Affective Incitement to Queer and Trans Studies in Education</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>In this chapter, the authors argue for “queer joy” as an affective incitement to extend and reconceptualize queer and trans studies across educational scholarship. Too often, research on queer and trans communities in PK-12 and higher education settings focuses on the discrimination, harassment, and violence that these groups face. Although this body of literature is important and needed to further advocate for more equitable practices and policies, the authors contend that queer and trans studies scholars must also document and examine how queer and trans communities create, experience, and proliferate queer joy in schools and other educational institutions. In this chapter, the authors draw analytical insights from feminist and queer of color critiques, and include excerpts from their discussions where they spoke about what PK-12 and higher education researchers can learn from one another about the conceptual and empirical possibilities of studying queer joy in education.</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1997-01-01</t>
+          <t>2023-04-12</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -3404,17 +3490,17 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004490123_036</t>
+          <t>https://doi.org/10.1163/9789004549791_010</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>595</t>
+          <t>109</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>595</t>
+          <t>124</t>
         </is>
       </c>
       <c r="S31" t="b">
@@ -3437,19 +3523,19 @@
         </is>
       </c>
       <c r="Z31">
-        <v>424</v>
+        <v>9</v>
       </c>
       <c r="AB31">
-        <v>1997</v>
+        <v>2023</v>
       </c>
       <c r="AC31" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W4327515011</t>
+          <t>https://api.openalex.org/works?filter=cites:W4381514609</t>
         </is>
       </c>
       <c r="AE31" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004490123_036</t>
+          <t>https://doi.org/10.1163/9789004549791_010</t>
         </is>
       </c>
       <c r="AF31" t="inlineStr">
@@ -3467,22 +3553,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://openalex.org/W600282006</t>
+          <t>https://openalex.org/W4229892663</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Poznań Studies in the Philosophy of the Sciences and the Humanities</t>
+          <t>Affirming Ambivalence</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Poznań Studies in the Philosophy of the Sciences and the Humanities</t>
+          <t>Affirming Ambivalence</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2001-01-01</t>
+          <t>2010-01-01</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -3502,17 +3588,17 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004457799_033</t>
+          <t>https://doi.org/10.1163/9789460911774_002</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>287</t>
+          <t>1</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>309</t>
+          <t>45</t>
         </is>
       </c>
       <c r="S32" t="b">
@@ -3535,19 +3621,19 @@
         </is>
       </c>
       <c r="Z32">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="AB32">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="AC32" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W600282006</t>
+          <t>https://api.openalex.org/works?filter=cites:W4229892663</t>
         </is>
       </c>
       <c r="AE32" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004457799_033</t>
+          <t>https://doi.org/10.1163/9789460911774_002</t>
         </is>
       </c>
       <c r="AF32" t="inlineStr">
@@ -3565,22 +3651,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://openalex.org/W2735160758</t>
+          <t>https://openalex.org/W4231826982</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Clitics, Morphological Merger, and the Mapping to Phonological Structure</t>
+          <t>THE OSSETIC CASE SYSTEM REVISITED</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Clitics, Morphological Merger, and the Mapping to Phonological Structure</t>
+          <t>THE OSSETIC CASE SYSTEM REVISITED</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1988-01-01</t>
+          <t>2008-01-01</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -3600,17 +3686,17 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004454101_017</t>
+          <t>https://doi.org/10.1163/9789401206358_008</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>253</t>
+          <t>87</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>270</t>
+          <t>105</t>
         </is>
       </c>
       <c r="S33" t="b">
@@ -3633,19 +3719,19 @@
         </is>
       </c>
       <c r="Z33">
-        <v>205</v>
+        <v>9</v>
       </c>
       <c r="AB33">
-        <v>1988</v>
+        <v>2008</v>
       </c>
       <c r="AC33" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W2735160758</t>
+          <t>https://api.openalex.org/works?filter=cites:W4231826982</t>
         </is>
       </c>
       <c r="AE33" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004454101_017</t>
+          <t>https://doi.org/10.1163/9789401206358_008</t>
         </is>
       </c>
       <c r="AF33" t="inlineStr">
@@ -3663,27 +3749,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://openalex.org/W784163460</t>
+          <t>https://openalex.org/W900935410</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>The Iberian Atlantic, 1492–2012</t>
+          <t>Filiation and Context: The Medieval Afterlife of the Policraticus</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>The Iberian Atlantic, 1492–2012</t>
+          <t>Filiation and Context: The Medieval Afterlife of the Policraticus</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>The Iberian Atlantic has a birth date. A perusal of the historical literature would suggest that the Iberian Atlantic has also a clear end. The circa 1500-1800 periodisation has two significant rationales. One is its association with early-modernity. The second rationale rests on the timing of European imperialism in the Americas and is equally valid despite the persistence of colonial rule in various specific areas of the Western Hemisphere. The density and breadth of the Iberian cultural influence in the Americas had two important consequences. One was that it made the Iberian Atlantic during the colonial period a socio-cultural space rather than simply a section of two empires, or of one during the union of the Spanish and Portuguese Crowns (1580-1640). The other is that it enabled the continuity of the Iberian Atlantic as a socio-cultural space long after it had ceased to exist as a political unit. Keywords: early-modernity; European imperialism; Iberian Atlantic; socio-cultural space; Western Hemisphere</t>
+          <t>Historians of political thought have long shown an interest in the reception of the Policraticus in the later Middle Ages. Walter Ullmann, Amnon Linder, Max Kerner and Thomas Elsmann have traced how knowledge of this great text was disseminated; they have also established a list of manuscripts, and mapped their geographical diffusion. Sometimes, John of Salisbury's text appeared under the title De nugis philosophorum . This chapter focuses on the enlargement of the readership of the Policraticus in the later Middle Ages, also with a special emphasis on its French component. The use of the metaphor of the body politic by John of Wales is also revealing of the mutation undergone by the text of John of Salisbury. In particular, Helinand seems to have been the principal mediator between John of Salisbury and the work undertaken by the Dominican Vincent of Beauvais. Keywords: Amnon Linder; Helinand; John of Salisbury; John of Wales; Max Kerner; Policraticus; Thomas Elsmann; Walter Ullmann</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2013-01-01</t>
+          <t>2014-12-02</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -3703,17 +3789,17 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004258068_005</t>
+          <t>https://doi.org/10.1163/9789004282940_014</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>375</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>73</t>
+          <t>438</t>
         </is>
       </c>
       <c r="S34" t="b">
@@ -3736,19 +3822,19 @@
         </is>
       </c>
       <c r="Z34">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AB34">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="AC34" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W784163460</t>
+          <t>https://api.openalex.org/works?filter=cites:W900935410</t>
         </is>
       </c>
       <c r="AE34" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004258068_005</t>
+          <t>https://doi.org/10.1163/9789004282940_014</t>
         </is>
       </c>
       <c r="AF34" t="inlineStr">
@@ -3766,27 +3852,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://openalex.org/W1547654455</t>
+          <t>https://openalex.org/W2775245034</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The Green Book of Language Revitalization in Practice</t>
+          <t>The “Global Turn” in Art History: Why, When, and How Does It Matter?</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>The Green Book of Language Revitalization in Practice</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Part I: Introduction L. Hinton, Language Revitalization: An Overview. A. Ash, J. Little Doe Fermino, and K. Hale, Diversity in Local Language Maintenance and Restoration: A Reason For Optimism. Part II: Language Policy L. Hinton, Federal Language Policy and Indigenous Languages in the United States. R.D. Arnold, ...To Help Assure the Survival and Continuing Vitality of Native American Part III: Language Planning L. Hinton, Language Planning. L. Hinton, Introduction to the Pueblo Languages. C.P. Sims, Native Language Planning: A Pilot Process in the Acoma Pueblo Community. R. Pecos and R. Blum-Martinez, The Key to Cultural Survival: Language Planning and Revitalization in the Pueblo de Cochiti. K. Hale, The Navajo Language: I. P.R. Platero, Navajo Head Start Language Study. Part IV: Maintenance And Revitalization of National Indigenous Languages L. Hinton, Introduction to Revitalization Of National Indigenous Languages. L. Hinton, Introduction to the Welsh Language. G. Morgan, Welsh: A European Case of Language Maintenance. K. Hale, Introduction to the Maori Language. J. King, Te Kohanga Reo: Maori Language Revitalization. L. Hinton, Introduction to the Hawaiian Language. S.L. No'eau Warner, The Movement to Revitalize Hawaiian Language and Culture. W.H. Wilson and K. Kamana, Loko Mai O Ka 'I'ini: Proceeding From A Dream - The 'Aha Punana Leo Connection In Hawaiian Language Revitalization. Part V: Immersion L. Hinton, Teaching Methods. L. Hinton, The Karuk Language. T. Supahan and S.E. Supahan, Teaching Well, Learning Quickly: Communication-Based Language Instruction. K. Hale, The Navajo Language: II. M. Arviso and W. Holm, Tsehootsooidi Olta'gi Dine Bizaad Bihoo'aah: A Navajo Immersion Program at Fort Defiance, Arizona. L. Hinton, The Master-Apprentice Language Learning Program. K. Hale, Linguistic Aspects of Language Teaching and Learning in Immersion Contexts. Part VI: Literacy L. Hinton, New Writing Systems. L. Hinton and K. Hale, An Introduction to Paiute. P. Bunte and R. Franklin, Language Revitalization in the San Juan Paiute Community and the Role of a Paiute Constitution. Part VII: Media and Technology L. Hinton, Audio-Video Documentation. K. Hale, Australian Languages. K. Hale, Strict Locality in Local Language Media: An Australian Example. K. Hale, The Arapaho Language. S. Greymorning, Reflections on the Arapaho Language Project, or When Bambi Spoke Arapaho and Other Tales of Arapaho Language Revitalization Efforts. K. Hale, Irish. C. Cotter, Continuity and Vitality: Expanding Domains through Irish-Language Radio. K. Hale, The Mono Language. P.V. Kroskrity and J.F. Reynolds, On Using Multimedia in Language Renewal: Observations from Making the CD-ROM Taitaduhaan. L. Buszard-Welcher, Can the Web Help Save My Language? Part VIII: Training L. Hinton, Training People to Teach Their Language. K. Hale, Inuttut and Innu-aimun. A. Johns and I. Mazurkewich, The Role of the University in the Training of Native Language Teachers: Labrador. L. Hinton, Languages of Arizona, Southern California, and Oklahoma. T.L. McCarty, L.J. Watahomigie, A.Y. Yamamoto, and O. Zepeda, Indigenous Educators as Change Agents: Case Studies of Two Language Institutes. K. Hale, The Navajo Language: III. C. Slate, Promoting Advanced Navajo Language Scholarship. Part IX: Sleeping Languages L. Hinton, Sleeping Languages: Can They Be Awakened? L. Hinton, The Use of Linguistic Archives in Language Revitalization: The Native California Language Restoration Workshop. L. Hinton, The Ohlone Languages. L. Yamane, New Life for a Lost Language. About the Editors. About the Authors. Index.</t>
+          <t>The “Global Turn” in Art History: Why, When, and How Does It Matter?</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2001-01-01</t>
+          <t>2017-01-01</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -3806,7 +3887,17 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004261723</t>
+          <t>https://doi.org/10.1163/9789004355798_013</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>299</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>313</t>
         </is>
       </c>
       <c r="S35" t="b">
@@ -3829,24 +3920,24 @@
         </is>
       </c>
       <c r="Z35">
-        <v>823</v>
+        <v>7</v>
       </c>
       <c r="AB35">
-        <v>2001</v>
+        <v>2017</v>
       </c>
       <c r="AC35" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W1547654455</t>
+          <t>https://api.openalex.org/works?filter=cites:W2775245034</t>
         </is>
       </c>
       <c r="AE35" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004261723</t>
+          <t>https://doi.org/10.1163/9789004355798_013</t>
         </is>
       </c>
       <c r="AF35" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>book-chapter</t>
         </is>
       </c>
       <c r="AI35" t="b">
@@ -3859,27 +3950,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://openalex.org/W188712711</t>
+          <t>https://openalex.org/W4385319205</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>A Companion to Boethius in the Middle Ages</t>
+          <t>Arabic and Islamic studies in honor of Hamilton A.R. Gibb</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>A Companion to Boethius in the Middle Ages</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>The articles in this volume focus upon Boethius's extant works: his De arithmetica and a fragmentary De musica, his translations and commentaries on logic, his five theological texts, and, of course, his Consolation of Philosophy. They examine the effects that Boethian thought has exercised upon the learning of later generations of scholars--including, to a degree, scholars of the 21st century. The field of Boethian Studies has enjoyed a continuous history of works that treat either the entire Boethian tradition or major aspects of it. This volume offers a comprehensive study, and its construction is systematic, considering Boethius's works both as central to the disciplines that they represent and to the areas of scholarly interest that they influenced, and it is framed by articles on the historical contexts in which those works were produced. Contributors include: Noel Harold Kaylor, Jr., Stephen McCluskey, Rosalind C. Love, Jean-Yves Guillaumin, Siobhan Nash-Marshall, John Casey, Paul E. Szarmach, Christine Hehle, Glynnis M. Cropp, Dario Bancato, Ian Johnson, Mark T. Rimple, Ann E. Moyer, Fabio Troncarelli, and Philip Edward Phillips.</t>
+          <t>Arabic and Islamic studies in honor of Hamilton A.R. Gibb</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2012-05-03</t>
+          <t>1965-01-01</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -3899,7 +3985,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004225381</t>
+          <t>https://doi.org/10.1163/9789004619159</t>
         </is>
       </c>
       <c r="S36" t="b">
@@ -3922,19 +4008,19 @@
         </is>
       </c>
       <c r="Z36">
-        <v>126</v>
+        <v>36</v>
       </c>
       <c r="AB36">
-        <v>2012</v>
+        <v>1965</v>
       </c>
       <c r="AC36" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W188712711</t>
+          <t>https://api.openalex.org/works?filter=cites:W4385319205</t>
         </is>
       </c>
       <c r="AE36" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004225381</t>
+          <t>https://doi.org/10.1163/9789004619159</t>
         </is>
       </c>
       <c r="AF36" t="inlineStr">
@@ -3952,27 +4038,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3199459961</t>
+          <t>https://openalex.org/W4248471311</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Hit like a Girl: Women Who Batter Their Partners</t>
+          <t>Collaborations between Mathematics Educators and Mathematicians for Mathematics Teacher Education in the United States</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Hit like a Girl: Women Who Batter Their Partners</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Domestic violence by women represents a blind spot for western society. Since 1977, multiple large scale international studies have demonstrated the women can and do beat, batter and murder their male and female intimate partners at a rate equal to or higher than that of man, yet this issue is not simply ignored but denied by society at large. Women's use of domestic violence is misrepresented by the media and denied by feminists, both of whom find the topic threatening. Despite this gender symmetry in domestic violence, media representations display male perpetrators 10 times more often than they display female perpetrators and when it is displayed, it is usually shown as humorous. For the media and the society it caters to, domestically violent women represent a failure of social control; women are not behaving in the expected manner. For feminists, domestically violent women threaten the victim paradigm upon which much of Second Wave feminism was based. This chapter will examine the prevalence of domestic violence by women against their intimate partners, exploring the societal myths and gender dogma that both hides and perpetuates this form of violence by women.</t>
+          <t>Collaborations between Mathematics Educators and Mathematicians for Mathematics Teacher Education in the United States</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2011-04-15</t>
+          <t>2019-12-02</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -3992,17 +4073,17 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9781848880740_027</t>
+          <t>https://doi.org/10.1163/9789004419230_007</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>153</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>283</t>
+          <t>181</t>
         </is>
       </c>
       <c r="S37" t="b">
@@ -4025,19 +4106,19 @@
         </is>
       </c>
       <c r="Z37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB37">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="AC37" t="inlineStr">
         <is>
-          <t>https://api.openalex.org/works?filter=cites:W3199459961</t>
+          <t>https://api.openalex.org/works?filter=cites:W4248471311</t>
         </is>
       </c>
       <c r="AE37" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9781848880740_027</t>
+          <t>https://doi.org/10.1163/9789004419230_007</t>
         </is>
       </c>
       <c r="AF37" t="inlineStr">
@@ -4055,22 +4136,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://openalex.org/W3015901506</t>
+          <t>https://openalex.org/W4241565509</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The Difference between Emergency Remote Teaching and Online Learning</t>
+          <t>Callimachus’ Muses</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>The Difference between Emergency Remote Teaching and Online Learning</t>
+          <t>Callimachus’ Muses</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>This paper examines the relationship Callimachus has with the Muses by investigating their role and function in a number of different texts, especially the Aetia. The Muses are an important way for poets to talk about the qualities of their own poetry and in Aetia 1–2 Callimachus builds on the depiction of the Muses in earlier poets and their capacity to provide inspiration or information to portray himself as participating in an active and engaged conversation with the individual Muses in turn. The individualized Muses in Aetia 1–2 reflect the ongoing process of specialization as to the province of each Muse which led to the traditional division into the ‘Muse of History’, etc. Callimachus did not persist with the framework of the Muse-dialogue in Aetia 3–4, but we should not think of Callimachus as therefore rejecting the Muses in Aetia 3–4, but as showing the relationship of poet to Muse from a different perspective from that in Aetia 1–2.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2024-09-25</t>
+          <t>2011-01-01</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -4090,68 +4176,1224 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>https://doi.org/10.1163/9789004702813_021</t>
+          <t>https://doi.org/10.1163/9789004216976_018</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>511</t>
+          <t>329</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>522</t>
+          <t>348</t>
         </is>
       </c>
       <c r="S38" t="b">
         <v>0</v>
       </c>
       <c r="T38" t="b">
+        <v>0</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W38" t="b">
+        <v>0</v>
+      </c>
+      <c r="X38" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z38">
+        <v>28</v>
+      </c>
+      <c r="AB38">
+        <v>2011</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W4241565509</t>
+        </is>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004216976_018</t>
+        </is>
+      </c>
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W4249381366</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Brill's Companion to Propertius</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Brill's Companion to Propertius</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2006-07-01</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835</t>
+        </is>
+      </c>
+      <c r="S39" t="b">
+        <v>0</v>
+      </c>
+      <c r="T39" t="b">
+        <v>0</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W39" t="b">
+        <v>0</v>
+      </c>
+      <c r="X39" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z39">
+        <v>106</v>
+      </c>
+      <c r="AB39">
+        <v>2006</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W4249381366</t>
+        </is>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835</t>
+        </is>
+      </c>
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="AI39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W624893779</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Brill's Companion to Callimachus</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Brill's Companion to Callimachus</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Few figures from Greco-Roman antiquity have undergone as much reassessment in recent decades as Callimachus of Cyrene, who was active at the Alexandrian court of the Ptolemies during the early third century BC. Once perceived as a supreme example of ivory tower detachment and abstruse learning, Callimachus has now come to be understood as an artificer of the images of a powerful and vibrant court and as a poet second only to Homer in his later reception. For the modern audience, the fragmentation of his texts and the diffusion of source materials has often impeded understanding his poetic achievement. Brill’s Companion to Callimachus has been designed to aid in negotiating this scholarly terrain, especially the process of editing and collecting his fragments, to illuminate his intellectual and social contexts, and to indicate the current directions that his scholarship is taking.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2011-07-27</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004216976</t>
+        </is>
+      </c>
+      <c r="S40" t="b">
+        <v>0</v>
+      </c>
+      <c r="T40" t="b">
+        <v>0</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W40" t="b">
+        <v>0</v>
+      </c>
+      <c r="X40" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z40">
+        <v>177</v>
+      </c>
+      <c r="AB40">
+        <v>2011</v>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W624893779</t>
+        </is>
+      </c>
+      <c r="AE40" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004216976</t>
+        </is>
+      </c>
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="AI40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W833910705</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Major Themes and Motifs in Propertius’ Love Poetry</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Major Themes and Motifs in Propertius’ Love Poetry</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2006-01-01</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_008</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="S41" t="b">
+        <v>0</v>
+      </c>
+      <c r="T41" t="b">
+        <v>0</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W41" t="b">
+        <v>0</v>
+      </c>
+      <c r="X41" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z41">
+        <v>65</v>
+      </c>
+      <c r="AB41">
+        <v>2006</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W833910705</t>
+        </is>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_008</t>
+        </is>
+      </c>
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W745394833</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Propertius and Hellenistic Poetry</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Propertius and Hellenistic Poetry</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2006-01-01</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_006</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="S42" t="b">
+        <v>0</v>
+      </c>
+      <c r="T42" t="b">
+        <v>0</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W42" t="b">
+        <v>0</v>
+      </c>
+      <c r="X42" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z42">
+        <v>51</v>
+      </c>
+      <c r="AB42">
+        <v>2006</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W745394833</t>
+        </is>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_006</t>
+        </is>
+      </c>
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W874904114</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>The Third Book: Defining a Poetic Self</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>The Third Book: Defining a Poetic Self</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2006-01-01</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_013</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>319</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>352</t>
+        </is>
+      </c>
+      <c r="S43" t="b">
+        <v>0</v>
+      </c>
+      <c r="T43" t="b">
+        <v>0</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W43" t="b">
+        <v>0</v>
+      </c>
+      <c r="X43" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z43">
+        <v>49</v>
+      </c>
+      <c r="AB43">
+        <v>2006</v>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W874904114</t>
+        </is>
+      </c>
+      <c r="AE43" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047404835_013</t>
+        </is>
+      </c>
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI43" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W828951668</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>The Amores: The Invention of Ovid</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>The Amores: The Invention of Ovid</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>This chapter uses literary and historical categories to provide a framework for the Amores . It looks at how Ovid invents a poetic identity for himself in the Amores . The most basic structural components of Ovid's elegiac book, juxtaposition and opposition, are techniques which Ovid also uses with poems that are less clearly to be considered pairs or thematic clusters. Ovid says that he is driven by a turbo ; one might go so far as to put Cupid in the role of a playful child, but Ovid does not explicitly do so. Uncertainty regarding the dating of the Amores ' composition is further complicated by the (presumably) separate matter of their publication. Even in his earliest literary incarnation, Ovid manages to elude the most earnest attempts to make him fit easy definition. Instead, he gives the reader Ouidius poeta , the Amores ' greatest, most versatile, and most dangerous invention. Keywords: Amores ; Cupid; Ovid; turbo</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2002-01-01</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047400950_004</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="S44" t="b">
+        <v>0</v>
+      </c>
+      <c r="T44" t="b">
+        <v>0</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W44" t="b">
+        <v>0</v>
+      </c>
+      <c r="X44" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z44">
+        <v>23</v>
+      </c>
+      <c r="AB44">
+        <v>2002</v>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W828951668</t>
+        </is>
+      </c>
+      <c r="AE44" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789047400950_004</t>
+        </is>
+      </c>
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI44" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W4247715605</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>The Origin of the Indo-Iranians</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>The Origin of the Indo-Iranians</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Here then is the fruit of Elena Kuz'mina's life-long quest for the Indo-Iranians. Already its predecessor (Otkuda prishli indoarii?, published in 1994) was considered the most comprehensive analysis of the origins of the Indo-Iranians ever published, but in this new, significantly expanded edition (edited by J.P. Mallory) we find an encyclopaedic account of the Andronovo culture of Eurasia. Taking its evidence from archaeology, linguistics, ethnology, mythology, and physical anthropology pertaining to Indo-Iranian origins and expansions, it comprehensively covers the relationships of this culture with neighboring areas and cultures, and its role in the foundation of the Indo-Iranian peoples.</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2007-06-22</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/ej.9789004160545.i-763</t>
+        </is>
+      </c>
+      <c r="S45" t="b">
+        <v>0</v>
+      </c>
+      <c r="T45" t="b">
+        <v>0</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W45" t="b">
+        <v>0</v>
+      </c>
+      <c r="X45" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z45">
+        <v>114</v>
+      </c>
+      <c r="AB45">
+        <v>2007</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W4247715605</t>
+        </is>
+      </c>
+      <c r="AE45" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/ej.9789004160545.i-763</t>
+        </is>
+      </c>
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="AI45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W2064220233</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Selected Writings on Chariots and other Early Vehicles, Riding and Harness</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Selected Writings on Chariots and other Early Vehicles, Riding and Harness</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>This collection of papers is primarily concerned with transport by wheeled vehicle in antiquity. They shed much light on the construction of the vehicles, the ways their draught animals were harnessed and controlled, and the uses to which the equipages were put. The evidence discussed includes actual remains of vehicles and bridles, as well as figured and textual documents. Ridden animals and their gear also feature in this collection of papers. The Selected Writings of Mary B. Littauer and Joost H. Crouwel are important for all those interested in the cultures of the ancient Near East, Egypt and Cyprus and of Bronze Age Greece.</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2002-01-01</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004494169</t>
+        </is>
+      </c>
+      <c r="S46" t="b">
+        <v>0</v>
+      </c>
+      <c r="T46" t="b">
+        <v>0</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W46" t="b">
+        <v>0</v>
+      </c>
+      <c r="X46" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z46">
+        <v>22</v>
+      </c>
+      <c r="AB46">
+        <v>2002</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W2064220233</t>
+        </is>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004494169</t>
+        </is>
+      </c>
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="AI46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W835497060</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>The Earliest Avar-Age Stirrups, Or The "Stirrup Controversy" Revisited</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>The Earliest Avar-Age Stirrups, Or The "Stirrup Controversy" Revisited</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>At the center of the was the question of whether technological innovation is a cause or an effect. In various articles, Bernard Bachrach has made it clear that although the stirrup became known in (western) Europe by A.D. 700, it had no military impact for another couple of centuries or more. Bachrach's conclusion was that the Avars may have known the device, but had no real use for it, since their combat techniques were mainly based on archery. This chapter corrects Bachrach's chronology and shows that, far from being isolated, the number of stirrup finds that could be dated before 650 is quite significant. The examination of the archaeological record of Early Avar-age burial assemblages has lent strong empirical support for the view that stirrups were symbolically associated to a class of professional warriors, who were often accompanied in death by their warhorses. Keywords: Bernard Bachrach; early Avar-age burial assemblages; stirrup controversy</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2008-01-01</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/ej.9789004163898.i-492.74</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>297</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>326</t>
+        </is>
+      </c>
+      <c r="S47" t="b">
+        <v>0</v>
+      </c>
+      <c r="T47" t="b">
+        <v>0</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W47" t="b">
+        <v>0</v>
+      </c>
+      <c r="X47" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z47">
+        <v>13</v>
+      </c>
+      <c r="AB47">
+        <v>2008</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W835497060</t>
+        </is>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/ej.9789004163898.i-492.74</t>
+        </is>
+      </c>
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W4212783537</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Social Class</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Social Class</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004505612_038</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>624</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>643</t>
+        </is>
+      </c>
+      <c r="S48" t="b">
+        <v>0</v>
+      </c>
+      <c r="T48" t="b">
+        <v>0</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>3</v>
+      </c>
+      <c r="AB48">
+        <v>2022</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W4212783537</t>
+        </is>
+      </c>
+      <c r="AE48" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004505612_038</t>
+        </is>
+      </c>
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI48" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W4212943639</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Alienation and Education</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Alienation and Education</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004505612_003</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="S49" t="b">
+        <v>0</v>
+      </c>
+      <c r="T49" t="b">
+        <v>0</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr">
+        <is>
+          <t>https://dora.dmu.ac.uk/handle/2086/21211</t>
+        </is>
+      </c>
+      <c r="W49" t="b">
         <v>1</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>green</t>
-        </is>
-      </c>
-      <c r="V38" t="inlineStr">
-        <is>
-          <t>https://vtechworks.lib.vt.edu/bitstream/10919/104648/1/facdev-article.pdf</t>
-        </is>
-      </c>
-      <c r="W38" t="b">
+      <c r="X49" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z49">
+        <v>2</v>
+      </c>
+      <c r="AB49">
+        <v>2022</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W4212943639</t>
+        </is>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004505612_003</t>
+        </is>
+      </c>
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>book-chapter</t>
+        </is>
+      </c>
+      <c r="AI49" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://openalex.org/W3169367280</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Marxism and Whiteness</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Marxism and Whiteness</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2020-11-28</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>BRILL eBooks</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://openalex.org/S4306462964</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Brill</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004444836_049</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>372</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>376</t>
+        </is>
+      </c>
+      <c r="S50" t="b">
+        <v>0</v>
+      </c>
+      <c r="T50" t="b">
+        <v>0</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>closed</t>
+        </is>
+      </c>
+      <c r="W50" t="b">
+        <v>0</v>
+      </c>
+      <c r="X50" t="inlineStr">
+        <is>
+          <t>en</t>
+        </is>
+      </c>
+      <c r="Z50">
         <v>1</v>
       </c>
-      <c r="X38" t="inlineStr">
-        <is>
-          <t>en</t>
-        </is>
-      </c>
-      <c r="Z38">
-        <v>4262</v>
-      </c>
-      <c r="AB38">
-        <v>2024</v>
-      </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>https://api.openalex.org/works?filter=cites:W3015901506</t>
-        </is>
-      </c>
-      <c r="AE38" t="inlineStr">
-        <is>
-          <t>https://doi.org/10.1163/9789004702813_021</t>
-        </is>
-      </c>
-      <c r="AF38" t="inlineStr">
+      <c r="AB50">
+        <v>2020</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>https://api.openalex.org/works?filter=cites:W3169367280</t>
+        </is>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t>https://doi.org/10.1163/9789004444836_049</t>
+        </is>
+      </c>
+      <c r="AF50" t="inlineStr">
         <is>
           <t>book-chapter</t>
         </is>
       </c>
-      <c r="AI38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ38" t="b">
+      <c r="AI50" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ50" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>